<commit_message>
writing, with errors - modified:   data/short.xlsx
</commit_message>
<xml_diff>
--- a/data/short.xlsx
+++ b/data/short.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Tlaltecuhtli/repos/GitHub/topa-development/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39604F12-6E4D-7841-9550-B230ACC8E9B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{913350EC-4596-7E4E-A54D-F1B98FECC402}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24140" windowHeight="12440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24040" windowHeight="10100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="provenance" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>AMANZI: The Multi-Process HPC Simulator</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Output path</t>
+  </si>
+  <si>
+    <t>=TEXT( G2"====================================================", "=" )</t>
   </si>
 </sst>
 </file>
@@ -198,11 +201,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -620,7 +624,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43439.731470226237</v>
+        <v>43439.761471684957</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -652,7 +656,7 @@
       </c>
       <c r="B17">
         <f ca="1">INFO( "numfile" )</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -679,7 +683,7 @@
       </c>
       <c r="B20" t="str">
         <f ca="1">INFO( "directory" )</f>
-        <v>/Users/l127914/Library/Containers/com.microsoft.Excel/Data/Documents/</v>
+        <v>/Volumes/Tlaltecuhtli/repos/GitHub/topa-development/data/</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -859,2060 +863,2752 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B231"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1">
+        <v>52</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <f>TEXT( "Amanzi XML Input Specification (Version 2.3-draft)", "=" )</f>
+        <v>Amanzi XML Input Specification (Version 2.3-draft)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4" t="str">
         <f>TEXT( "====================================================", "=" )</f>
         <v>====================================================</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f>TEXT( "Amanzi XML Input Specification (Version 2.3-draft)", "=" )</f>
-        <v>Amanzi XML Input Specification (Version 2.3-draft)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f>TEXT( "====================================================", "=" )</f>
-        <v>====================================================</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4" t="str">
         <f>TEXT( ".. contents:: **Table of Contents**", "=" )</f>
         <v>.. contents:: **Table of Contents**</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="str">
         <f>TEXT( "Overview", "=" )</f>
         <v>Overview</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="str">
         <f>TEXT( "========", "=" )</f>
         <v>========</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>619</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>532</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4" t="str">
         <f>TEXT( "Amanzi Input", "=" )</f>
         <v>Amanzi Input</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18" s="4" t="str">
         <f>TEXT( "============", "=" )</f>
         <v>============</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>493</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>883</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>803</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="str">
+      <c r="B26">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="str">
         <f>TEXT( "An example root tag of an input file would look like the following.", "=" )</f>
         <v>An example root tag of an input file would look like the following.</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="str">
+      <c r="B28">
+        <v>19</v>
+      </c>
+      <c r="C28" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B33">
+        <v>17</v>
+      </c>
+      <c r="C33" s="4" t="str">
         <f>TEXT( "Model Description", "=" )</f>
         <v>Model Description</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34">
+        <v>17</v>
+      </c>
+      <c r="C34" s="4" t="str">
         <f>TEXT( "=================", "=" )</f>
         <v>=================</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B36">
+        <v>227</v>
+      </c>
+      <c r="C36" s="4" t="str">
         <f>TEXT( "This allows the users to provide a name and general description of model being developed.  This is also the section in which the units for the problem are stored. This entire section is optional but encouraged as documentation.", "=" )</f>
         <v>This allows the users to provide a name and general description of model being developed.  This is also the section in which the units for the problem are stored. This entire section is optional but encouraged as documentation.</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B38">
+        <v>19</v>
+      </c>
+      <c r="C38" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="str">
+      <c r="B41">
+        <v>29</v>
+      </c>
+      <c r="C41" s="4" t="str">
         <f>TEXT( "      Required Elements: NONE", "=" )</f>
         <v xml:space="preserve">      Required Elements: NONE</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="str">
+      <c r="B42">
+        <v>98</v>
+      </c>
+      <c r="C42" s="4" t="str">
         <f>TEXT( "      Optional Elements: comment, author, created, modified, model_id, description, purpose, units", "=" )</f>
         <v xml:space="preserve">      Optional Elements: comment, author, created, modified, model_id, description, purpose, units</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="str">
+      <c r="B43">
+        <v>22</v>
+      </c>
+      <c r="C43" s="4" t="str">
         <f>TEXT( "  &lt;/model_description&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/model_description&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" t="str">
+      <c r="B45">
+        <v>78</v>
+      </c>
+      <c r="C45" s="4" t="str">
         <f>TEXT( "All elements expect string content, except ``units`` which is described below.", "=" )</f>
         <v>All elements expect string content, except ``units`` which is described below.</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" t="str">
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" s="4" t="str">
         <f>TEXT( "Units", "=" )</f>
         <v>Units</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" t="str">
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48" s="4" t="str">
         <f>TEXT( "-----", "=" )</f>
         <v>-----</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+        <v>463</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" t="str">
+      <c r="B52">
+        <v>158</v>
+      </c>
+      <c r="C52" s="4" t="str">
         <f>TEXT( "``units`` has the optional elements of length, time, mass, and concentration.  Each of those in turn have their own structure.  The structures are as follows.", "=" )</f>
         <v>``units`` has the optional elements of length, time, mass, and concentration.  Each of those in turn have their own structure.  The structures are as follows.</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" t="str">
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54" s="4" t="str">
         <f>TEXT( "REMINDER - UNITS ARE NOT IMPLEMENTED YET", "=" )</f>
         <v>REMINDER - UNITS ARE NOT IMPLEMENTED YET</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" t="str">
+      <c r="B56">
+        <v>19</v>
+      </c>
+      <c r="C56" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" t="str">
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58" s="4" t="str">
         <f>TEXT( "  &lt;units&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;units&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" t="str">
+      <c r="B59">
+        <v>29</v>
+      </c>
+      <c r="C59" s="4" t="str">
         <f>TEXT( "      Required Elements: NONE", "=" )</f>
         <v xml:space="preserve">      Required Elements: NONE</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" t="str">
+      <c r="B60">
+        <v>69</v>
+      </c>
+      <c r="C60" s="4" t="str">
         <f>TEXT( "      Optional Elements: length_unit, time_unit, mass_unit, conc_unit", "=" )</f>
         <v xml:space="preserve">      Optional Elements: length_unit, time_unit, mass_unit, conc_unit</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" t="str">
+      <c r="B61">
+        <v>10</v>
+      </c>
+      <c r="C61" s="4" t="str">
         <f>TEXT( "  &lt;/units&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/units&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" t="str">
+      <c r="B63">
+        <v>47</v>
+      </c>
+      <c r="C63" s="4" t="str">
         <f>TEXT( "Acceptable values for each unit are as follows:", "=" )</f>
         <v>Acceptable values for each unit are as follows:</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" t="str">
+      <c r="B65">
+        <v>35</v>
+      </c>
+      <c r="C65" s="4" t="str">
         <f>TEXT( "+----------------+----------------+", "=" )</f>
         <v>+----------------+----------------+</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" t="str">
+      <c r="B66">
+        <v>35</v>
+      </c>
+      <c r="C66" s="4" t="str">
         <f>TEXT( "| Units Elements | Value Options  |", "=" )</f>
         <v>| Units Elements | Value Options  |</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" t="str">
+      <c r="B67">
+        <v>35</v>
+      </c>
+      <c r="C67" s="4" t="str">
         <f>TEXT( "+================+================+", "=" )</f>
         <v>+================+================+</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" t="str">
+      <c r="B68">
+        <v>35</v>
+      </c>
+      <c r="C68" s="4" t="str">
         <f>TEXT( "| length_unit    | m or cm        |", "=" )</f>
         <v>| length_unit    | m or cm        |</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" t="str">
+      <c r="B69">
+        <v>35</v>
+      </c>
+      <c r="C69" s="4" t="str">
         <f>TEXT( "+----------------+----------------+", "=" )</f>
         <v>+----------------+----------------+</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" t="str">
+      <c r="B70">
+        <v>35</v>
+      </c>
+      <c r="C70" s="4" t="str">
         <f>TEXT( "| time_unit      | y, d, h, or s  |", "=" )</f>
         <v>| time_unit      | y, d, h, or s  |</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" t="str">
+      <c r="B71">
+        <v>35</v>
+      </c>
+      <c r="C71" s="4" t="str">
         <f>TEXT( "+----------------+----------------+", "=" )</f>
         <v>+----------------+----------------+</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" t="str">
+      <c r="B72">
+        <v>35</v>
+      </c>
+      <c r="C72" s="4" t="str">
         <f>TEXT( "| mass_unit      | kg             |", "=" )</f>
         <v>| mass_unit      | kg             |</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" t="str">
+      <c r="B73">
+        <v>35</v>
+      </c>
+      <c r="C73" s="4" t="str">
         <f>TEXT( "+----------------+----------------+", "=" )</f>
         <v>+----------------+----------------+</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" t="str">
+      <c r="B74">
+        <v>35</v>
+      </c>
+      <c r="C74" s="4" t="str">
         <f>TEXT( "| conc_unit      | molar, SI      |", "=" )</f>
         <v>| conc_unit      | molar, SI      |</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" t="str">
+      <c r="B75">
+        <v>35</v>
+      </c>
+      <c r="C75" s="4" t="str">
         <f>TEXT( "+----------------+----------------+", "=" )</f>
         <v>+----------------+----------------+</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" t="str">
+      <c r="B77">
+        <v>169</v>
+      </c>
+      <c r="C77" s="4" t="str">
         <f>TEXT( "Note, currently mol/m^3 concentration unit is only available for unstructured.  The input converter for unstructured will convert the concentration internally as needed.", "=" )</f>
         <v>Note, currently mol/m^3 concentration unit is only available for unstructured.  The input converter for unstructured will convert the concentration internally as needed.</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" t="str">
+      <c r="B79">
+        <v>61</v>
+      </c>
+      <c r="C79" s="4" t="str">
         <f>TEXT( "Here is an overall example for the model description element.", "=" )</f>
         <v>Here is an overall example for the model description element.</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81" t="str">
+      <c r="B81">
+        <v>19</v>
+      </c>
+      <c r="C81" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" t="str">
+      <c r="B84">
+        <v>103</v>
+      </c>
+      <c r="C84" s="4" t="str">
         <f>TEXT( "    &lt;comments&gt;This is a simplified 3-layer DVZ problem in 2D with two cribs (Flow+Transport)&lt;/comments&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;comments&gt;This is a simplified 3-layer DVZ problem in 2D with two cribs (Flow+Transport)&lt;/comments&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" t="str">
+      <c r="B85">
+        <v>39</v>
+      </c>
+      <c r="C85" s="4" t="str">
         <f>TEXT( "    &lt;model_name&gt;DVZ 3layer&lt;/model_name&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;model_name&gt;DVZ 3layer&lt;/model_name&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" t="str">
+      <c r="B86">
+        <v>27</v>
+      </c>
+      <c r="C86" s="4" t="str">
         <f>TEXT( "    &lt;author&gt;d3k870&lt;/author&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;author&gt;d3k870&lt;/author&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" t="str">
+      <c r="B87">
+        <v>11</v>
+      </c>
+      <c r="C87" s="4" t="str">
         <f>TEXT( "    &lt;units&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;units&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88" t="str">
+      <c r="B88">
+        <v>34</v>
+      </c>
+      <c r="C88" s="4" t="str">
         <f>TEXT( "      &lt;length_unit&gt;m&lt;/length_unit&gt;", "=" )</f>
         <v xml:space="preserve">      &lt;length_unit&gt;m&lt;/length_unit&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89" t="str">
+      <c r="B89">
+        <v>30</v>
+      </c>
+      <c r="C89" s="4" t="str">
         <f>TEXT( "      &lt;time_unit&gt;s&lt;/time_unit&gt;", "=" )</f>
         <v xml:space="preserve">      &lt;time_unit&gt;s&lt;/time_unit&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" t="str">
+      <c r="B90">
+        <v>31</v>
+      </c>
+      <c r="C90" s="4" t="str">
         <f>TEXT( "      &lt;mass_unit&gt;kg&lt;/mass_unit&gt;", "=" )</f>
         <v xml:space="preserve">      &lt;mass_unit&gt;kg&lt;/mass_unit&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" t="str">
+      <c r="B91">
+        <v>34</v>
+      </c>
+      <c r="C91" s="4" t="str">
         <f>TEXT( "      &lt;conc_unit&gt;molar&lt;/conc_unit&gt;", "=" )</f>
         <v xml:space="preserve">      &lt;conc_unit&gt;molar&lt;/conc_unit&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" t="str">
+      <c r="B92">
+        <v>12</v>
+      </c>
+      <c r="C92" s="4" t="str">
         <f>TEXT( "    &lt;/units&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;/units&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" t="str">
+      <c r="B93">
+        <v>22</v>
+      </c>
+      <c r="C93" s="4" t="str">
         <f>TEXT( "  &lt;/model_description&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/model_description&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" t="str">
+      <c r="B96">
+        <v>11</v>
+      </c>
+      <c r="C96" s="4" t="str">
         <f>TEXT( "Definitions", "=" )</f>
         <v>Definitions</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97" t="str">
+      <c r="B97">
+        <v>11</v>
+      </c>
+      <c r="C97" s="4" t="str">
         <f>TEXT( "===========", "=" )</f>
         <v>===========</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+      <c r="C99" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
-      <c r="B100" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" t="str">
+      <c r="B101">
+        <v>19</v>
+      </c>
+      <c r="C101" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
-      <c r="B102" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
-      <c r="B103" t="str">
+      <c r="B103">
+        <v>15</v>
+      </c>
+      <c r="C103" s="4" t="str">
         <f>TEXT( "  &lt;definitions&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;definitions&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
-      <c r="B104" t="str">
+      <c r="B104">
+        <v>29</v>
+      </c>
+      <c r="C104" s="4" t="str">
         <f>TEXT( "      Required Elements: NONE", "=" )</f>
         <v xml:space="preserve">      Required Elements: NONE</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
-      <c r="B105" t="str">
+      <c r="B105">
+        <v>42</v>
+      </c>
+      <c r="C105" s="4" t="str">
         <f>TEXT( "      Optional Elements: constants, macros", "=" )</f>
         <v xml:space="preserve">      Optional Elements: constants, macros</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
-      <c r="B106" t="str">
+      <c r="B106">
+        <v>16</v>
+      </c>
+      <c r="C106" s="4" t="str">
         <f>TEXT( "  &lt;/definitions&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/definitions&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
-      <c r="B107" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
-      <c r="B108" t="str">
+      <c r="B108">
+        <v>9</v>
+      </c>
+      <c r="C108" s="4" t="str">
         <f>TEXT( "Constants", "=" )</f>
         <v>Constants</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109" t="str">
+      <c r="B109">
+        <v>9</v>
+      </c>
+      <c r="C109" s="4" t="str">
         <f>TEXT( "---------", "=" )</f>
         <v>---------</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
-      <c r="B110" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="C111" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
-      <c r="B112" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
-      <c r="B113" t="str">
+      <c r="B113">
+        <v>19</v>
+      </c>
+      <c r="C113" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
-      <c r="B114" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
-      <c r="B115" t="str">
+      <c r="B115">
+        <v>13</v>
+      </c>
+      <c r="C115" s="4" t="str">
         <f>TEXT( "  &lt;constants&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;constants&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
-      <c r="B116" t="str">
+      <c r="B116">
+        <v>29</v>
+      </c>
+      <c r="C116" s="4" t="str">
         <f>TEXT( "      Required Elements: NONE", "=" )</f>
         <v xml:space="preserve">      Required Elements: NONE</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
-      <c r="B117" t="str">
+      <c r="B117">
+        <v>93</v>
+      </c>
+      <c r="C117" s="4" t="str">
         <f>TEXT( "      Optional Elements: constant, time_constant, numerical_constant, area_mass_flux_constant", "=" )</f>
         <v xml:space="preserve">      Optional Elements: constant, time_constant, numerical_constant, area_mass_flux_constant</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
-      <c r="B118" t="str">
+      <c r="B118">
+        <v>14</v>
+      </c>
+      <c r="C118" s="4" t="str">
         <f>TEXT( "  &lt;/constants&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/constants&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
-      <c r="B119" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>0</v>
+      </c>
+      <c r="C119" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+      <c r="C120" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
-      <c r="B121" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
-      <c r="B122" t="str">
+      <c r="B122">
+        <v>19</v>
+      </c>
+      <c r="C122" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
-      <c r="B123" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
       <c r="B124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="C124" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
-      <c r="B125" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
-      <c r="B126" t="str">
+      <c r="B126">
+        <v>186</v>
+      </c>
+      <c r="C126" s="4" t="str">
         <f>TEXT( "A ``time_constant`` is a specific form of a constant assuming the constant type is a time.  It takes the attributes ``name`` and ``value`` where the value is a time (time unit optional).", "=" )</f>
         <v>A ``time_constant`` is a specific form of a constant assuming the constant type is a time.  It takes the attributes ``name`` and ``value`` where the value is a time (time unit optional).</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
-      <c r="B127" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>0</v>
+      </c>
+      <c r="C127" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
-      <c r="B128" t="str">
+      <c r="B128">
+        <v>19</v>
+      </c>
+      <c r="C128" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
-      <c r="B129" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>0</v>
+      </c>
+      <c r="C129" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="C130" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
-      <c r="B131" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
-      <c r="B132" t="str">
+      <c r="B132">
+        <v>107</v>
+      </c>
+      <c r="C132" s="4" t="str">
         <f>TEXT( "A ``numerical_constant`` is a specific form of a constant.  It takes the attributes ``name`` and ``value``.", "=" )</f>
         <v>A ``numerical_constant`` is a specific form of a constant.  It takes the attributes ``name`` and ``value``.</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
-      <c r="B133" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>0</v>
+      </c>
+      <c r="C133" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
-      <c r="B134" t="str">
+      <c r="B134">
+        <v>19</v>
+      </c>
+      <c r="C134" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
-      <c r="B135" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>0</v>
+      </c>
+      <c r="C135" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
       <c r="B136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+      <c r="C136" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
-      <c r="B137" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
-      <c r="B138" t="str">
+      <c r="B138">
+        <v>149</v>
+      </c>
+      <c r="C138" s="4" t="str">
         <f>TEXT( "A ``area_mass_flux_constant`` is a specific form of a constant.  It takes the attributes ``name`` and ``value`` where the value is an area mass flux.", "=" )</f>
         <v>A ``area_mass_flux_constant`` is a specific form of a constant.  It takes the attributes ``name`` and ``value`` where the value is an area mass flux.</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
-      <c r="B139" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
-      <c r="B140" t="str">
+      <c r="B140">
+        <v>19</v>
+      </c>
+      <c r="C140" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
-      <c r="B141" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>0</v>
+      </c>
+      <c r="C141" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
       <c r="B142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="C142" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
-      <c r="B143" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
-      <c r="B144" t="str">
+      <c r="B144">
+        <v>6</v>
+      </c>
+      <c r="C144" s="4" t="str">
         <f>TEXT( "Macros", "=" )</f>
         <v>Macros</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
-      <c r="B145" t="str">
+      <c r="B145">
+        <v>6</v>
+      </c>
+      <c r="C145" s="4" t="str">
         <f>TEXT( "------", "=" )</f>
         <v>------</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
-      <c r="B146" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
-      <c r="B147" t="str">
+      <c r="B147">
+        <v>210</v>
+      </c>
+      <c r="C147" s="4" t="str">
         <f>TEXT( "The ``macros`` section defines time, cycle, and variable macros.  These specify a list or interval for triggering an action, particularly, writing out visualization, checkpoint, walkabout, or observation files.", "=" )</f>
         <v>The ``macros`` section defines time, cycle, and variable macros.  These specify a list or interval for triggering an action, particularly, writing out visualization, checkpoint, walkabout, or observation files.</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
-      <c r="B148" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
-      <c r="B149" t="str">
+      <c r="B149">
+        <v>19</v>
+      </c>
+      <c r="C149" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
-      <c r="B150" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
-      <c r="B151" t="str">
+      <c r="B151">
+        <v>13</v>
+      </c>
+      <c r="C151" s="4" t="str">
         <f>TEXT( "  &lt;constants&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;constants&gt;</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
-      <c r="B152" t="str">
+      <c r="B152">
+        <v>29</v>
+      </c>
+      <c r="C152" s="4" t="str">
         <f>TEXT( "      Required Elements: NONE", "=" )</f>
         <v xml:space="preserve">      Required Elements: NONE</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
-      <c r="B153" t="str">
+      <c r="B153">
+        <v>68</v>
+      </c>
+      <c r="C153" s="4" t="str">
         <f>TEXT( "      Optional Elements: time_macro, cycle_macro, variable_macro [S]", "=" )</f>
         <v xml:space="preserve">      Optional Elements: time_macro, cycle_macro, variable_macro [S]</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
-      <c r="B154" t="str">
+      <c r="B154">
+        <v>14</v>
+      </c>
+      <c r="C154" s="4" t="str">
         <f>TEXT( "  &lt;/constants&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/constants&gt;</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
-      <c r="B155" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
-      <c r="B156" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
-      <c r="B157" t="str">
+      <c r="B157">
+        <v>10</v>
+      </c>
+      <c r="C157" s="4" t="str">
         <f>TEXT( "Time_macro", "=" )</f>
         <v>Time_macro</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
-      <c r="B158" t="str">
+      <c r="B158">
+        <v>10</v>
+      </c>
+      <c r="C158" s="4" t="str">
         <f>TEXT( "__________", "=" )</f>
         <v>__________</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
-      <c r="B159" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
       <c r="B160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+      <c r="C160" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
-      <c r="B161" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
-      <c r="B162" t="str">
+      <c r="B162">
+        <v>19</v>
+      </c>
+      <c r="C162" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
-      <c r="B163" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B163">
+        <v>0</v>
+      </c>
+      <c r="C163" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="C164" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
-      <c r="B165" t="str">
+      <c r="B165">
+        <v>22</v>
+      </c>
+      <c r="C165" s="4" t="str">
         <f>TEXT( "    &lt;time&gt;Value&lt;/time&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;time&gt;Value&lt;/time&gt;</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
-      <c r="B166" t="str">
+      <c r="B166">
+        <v>15</v>
+      </c>
+      <c r="C166" s="4" t="str">
         <f>TEXT( "  &lt;/time_macro&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/time_macro&gt;</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
-      <c r="B167" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
-      <c r="B168" t="str">
+      <c r="B168">
+        <v>2</v>
+      </c>
+      <c r="C168" s="4" t="str">
         <f>TEXT( "or", "=" )</f>
         <v>or</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
-      <c r="B169" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
-      <c r="B170" t="str">
+      <c r="B170">
+        <v>19</v>
+      </c>
+      <c r="C170" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
-      <c r="B171" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
       <c r="B172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="C172" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
-      <c r="B173" t="str">
+      <c r="B173">
+        <v>30</v>
+      </c>
+      <c r="C173" s="4" t="str">
         <f>TEXT( "    &lt;start&gt; TimeValue &lt;/start&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;start&gt; TimeValue &lt;/start&gt;</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
-      <c r="B174" t="str">
+      <c r="B174">
+        <v>62</v>
+      </c>
+      <c r="C174" s="4" t="str">
         <f>TEXT( "    &lt;timestep_interval&gt; TimeIntervalValue &lt;/timestep_interval&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;timestep_interval&gt; TimeIntervalValue &lt;/timestep_interval&gt;</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
-      <c r="B175" t="str">
+      <c r="B175">
+        <v>33</v>
+      </c>
+      <c r="C175" s="4" t="str">
         <f>TEXT( "    &lt;stop&gt; TimeValue | -1 &lt;/stop&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;stop&gt; TimeValue | -1 &lt;/stop&gt;</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
-      <c r="B176" t="str">
+      <c r="B176">
+        <v>15</v>
+      </c>
+      <c r="C176" s="4" t="str">
         <f>TEXT( "  &lt;/time_macro&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/time_macro&gt;</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
-      <c r="B177" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
-      <c r="B178" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
-      <c r="B179" t="str">
+      <c r="B179">
+        <v>11</v>
+      </c>
+      <c r="C179" s="4" t="str">
         <f>TEXT( "Cycle_macro", "=" )</f>
         <v>Cycle_macro</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
-      <c r="B180" t="str">
+      <c r="B180">
+        <v>11</v>
+      </c>
+      <c r="C180" s="4" t="str">
         <f>TEXT( "___________", "=" )</f>
         <v>___________</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
-      <c r="B181" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
-      <c r="B182" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B182">
+        <v>0</v>
+      </c>
+      <c r="C182" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
-      <c r="B183" t="str">
+      <c r="B183">
+        <v>225</v>
+      </c>
+      <c r="C183" s="4" t="str">
         <f>TEXT( "The ``cycle_macro`` requires an attribute ``name`` and the subelements ``start``, ``timestep_interval``, and ``stop`` with integer values.  A ``stop`` value of -1 will continue the cycle macro until the end of the simulation.", "=" )</f>
         <v>The ``cycle_macro`` requires an attribute ``name`` and the subelements ``start``, ``timestep_interval``, and ``stop`` with integer values.  A ``stop`` value of -1 will continue the cycle macro until the end of the simulation.</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
-      <c r="B184" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
-      <c r="B185" t="str">
+      <c r="B185">
+        <v>19</v>
+      </c>
+      <c r="C185" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
-      <c r="B186" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="C186" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
       <c r="B187">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="C187" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
-      <c r="B188" t="str">
+      <c r="B188">
+        <v>24</v>
+      </c>
+      <c r="C188" s="4" t="str">
         <f>TEXT( "    &lt;start&gt;Value&lt;/start&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;start&gt;Value&lt;/start&gt;</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
-      <c r="B189" t="str">
+      <c r="B189">
+        <v>48</v>
+      </c>
+      <c r="C189" s="4" t="str">
         <f>TEXT( "    &lt;timestep_interval&gt;Value&lt;/timestep_interval&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;timestep_interval&gt;Value&lt;/timestep_interval&gt;</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
-      <c r="B190" t="str">
+      <c r="B190">
+        <v>25</v>
+      </c>
+      <c r="C190" s="4" t="str">
         <f>TEXT( "    &lt;stop&gt;Value|-1&lt;/stop&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;stop&gt;Value|-1&lt;/stop&gt;</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
-      <c r="B191" t="str">
+      <c r="B191">
+        <v>16</v>
+      </c>
+      <c r="C191" s="4" t="str">
         <f>TEXT( "  &lt;/cycle_macro&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/cycle_macro&gt;</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
-      <c r="B192" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
-      <c r="B193" t="str">
+      <c r="B193">
+        <v>14</v>
+      </c>
+      <c r="C193" s="4" t="str">
         <f>TEXT( "Variable_macro", "=" )</f>
         <v>Variable_macro</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
-      <c r="B194" t="str">
+      <c r="B194">
+        <v>14</v>
+      </c>
+      <c r="C194" s="4" t="str">
         <f>TEXT( "______________", "=" )</f>
         <v>______________</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
-      <c r="B195" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
-      <c r="B196" t="str">
+      <c r="B196">
+        <v>115</v>
+      </c>
+      <c r="C196" s="4" t="str">
         <f>TEXT( "The ``variable_macro`` requires an attribute ``name``  and one or more subelements ``variable`` containing strings.", "=" )</f>
         <v>The ``variable_macro`` requires an attribute ``name``  and one or more subelements ``variable`` containing strings.</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
-      <c r="B197" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
-      <c r="B198" t="str">
+      <c r="B198">
+        <v>19</v>
+      </c>
+      <c r="C198" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
-      <c r="B199" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B199">
+        <v>0</v>
+      </c>
+      <c r="C199" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
       <c r="B200">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="C200" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
-      <c r="B201" t="str">
+      <c r="B201">
+        <v>41</v>
+      </c>
+      <c r="C201" s="4" t="str">
         <f>TEXT( "    &lt;variable&gt; VariableString &lt;/variable&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;variable&gt; VariableString &lt;/variable&gt;</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
-      <c r="B202" t="str">
+      <c r="B202">
+        <v>19</v>
+      </c>
+      <c r="C202" s="4" t="str">
         <f>TEXT( "  &lt;/variable_macro&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/variable_macro&gt;</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
-      <c r="B203" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
-      <c r="B204" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B204">
+        <v>0</v>
+      </c>
+      <c r="C204" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
-      <c r="B205" t="str">
+      <c r="B205">
+        <v>62</v>
+      </c>
+      <c r="C205" s="4" t="str">
         <f>TEXT( "An example ``definition`` section would look as the following:", "=" )</f>
         <v>An example ``definition`` section would look as the following:</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>205</v>
       </c>
-      <c r="B206" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B206">
+        <v>0</v>
+      </c>
+      <c r="C206" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>206</v>
       </c>
-      <c r="B207" t="str">
+      <c r="B207">
+        <v>19</v>
+      </c>
+      <c r="C207" s="4" t="str">
         <f>TEXT( ".. code-block:: xml", "=" )</f>
         <v>.. code-block:: xml</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>207</v>
       </c>
-      <c r="B208" t="str">
-        <f>TEXT( "", "=" )</f>
-        <v/>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B208">
+        <v>0</v>
+      </c>
+      <c r="C208" s="4" t="str">
+        <f>TEXT( "", "=" )</f>
+        <v/>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>208</v>
       </c>
-      <c r="B209" t="str">
+      <c r="B209">
+        <v>15</v>
+      </c>
+      <c r="C209" s="4" t="str">
         <f>TEXT( "  &lt;definitions&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;definitions&gt;</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>209</v>
       </c>
-      <c r="B210" t="str">
+      <c r="B210">
+        <v>15</v>
+      </c>
+      <c r="C210" s="4" t="str">
         <f>TEXT( "    &lt;constants&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;constants&gt;</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>210</v>
       </c>
       <c r="B211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="C211" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>211</v>
       </c>
       <c r="B212">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="C212" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>212</v>
       </c>
       <c r="B213">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="C213" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>213</v>
       </c>
       <c r="B214">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="C214" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>214</v>
       </c>
       <c r="B215">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="C215" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>215</v>
       </c>
-      <c r="B216" t="str">
+      <c r="B216">
+        <v>16</v>
+      </c>
+      <c r="C216" s="4" t="str">
         <f>TEXT( "    &lt;/constants&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;/constants&gt;</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>216</v>
       </c>
-      <c r="B217" t="str">
+      <c r="B217">
+        <v>12</v>
+      </c>
+      <c r="C217" s="4" t="str">
         <f>TEXT( "    &lt;macros&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;macros&gt;</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>217</v>
       </c>
       <c r="B218">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="C218" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>218</v>
       </c>
-      <c r="B219" t="str">
+      <c r="B219">
+        <v>34</v>
+      </c>
+      <c r="C219" s="4" t="str">
         <f>TEXT( "        &lt;time&gt;6.17266656E10&lt;/time&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;time&gt;6.17266656E10&lt;/time&gt;</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>219</v>
       </c>
-      <c r="B220" t="str">
+      <c r="B220">
+        <v>35</v>
+      </c>
+      <c r="C220" s="4" t="str">
         <f>TEXT( "        &lt;time&gt;6.172982136E10&lt;/time&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;time&gt;6.172982136E10&lt;/time&gt;</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>220</v>
       </c>
-      <c r="B221" t="str">
+      <c r="B221">
+        <v>35</v>
+      </c>
+      <c r="C221" s="4" t="str">
         <f>TEXT( "        &lt;time&gt;6.173297712E10&lt;/time&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;time&gt;6.173297712E10&lt;/time&gt;</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>221</v>
       </c>
-      <c r="B222" t="str">
+      <c r="B222">
+        <v>36</v>
+      </c>
+      <c r="C222" s="4" t="str">
         <f>TEXT( "        &lt;time&gt;6.3372710016E10&lt;/time&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;time&gt;6.3372710016E10&lt;/time&gt;</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>222</v>
       </c>
-      <c r="B223" t="str">
+      <c r="B223">
+        <v>34</v>
+      </c>
+      <c r="C223" s="4" t="str">
         <f>TEXT( "        &lt;time&gt;6.33834396E10&lt;/time&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;time&gt;6.33834396E10&lt;/time&gt;</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>223</v>
       </c>
-      <c r="B224" t="str">
+      <c r="B224">
+        <v>19</v>
+      </c>
+      <c r="C224" s="4" t="str">
         <f>TEXT( "      &lt;/time_macro&gt;", "=" )</f>
         <v xml:space="preserve">      &lt;/time_macro&gt;</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>224</v>
       </c>
       <c r="B225">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="C225" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>225</v>
       </c>
-      <c r="B226" t="str">
+      <c r="B226">
+        <v>24</v>
+      </c>
+      <c r="C226" s="4" t="str">
         <f>TEXT( "        &lt;start&gt;0&lt;/start&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;start&gt;0&lt;/start&gt;</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>226</v>
       </c>
-      <c r="B227" t="str">
+      <c r="B227">
+        <v>51</v>
+      </c>
+      <c r="C227" s="4" t="str">
         <f>TEXT( "        &lt;timestep_interval&gt;1000&lt;/timestep_interval&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;timestep_interval&gt;1000&lt;/timestep_interval&gt;</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>227</v>
       </c>
-      <c r="B228" t="str">
+      <c r="B228">
+        <v>24</v>
+      </c>
+      <c r="C228" s="4" t="str">
         <f>TEXT( "        &lt;stop&gt;-1 &lt;/stop&gt;", "=" )</f>
         <v xml:space="preserve">        &lt;stop&gt;-1 &lt;/stop&gt;</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>228</v>
       </c>
-      <c r="B229" t="str">
+      <c r="B229">
+        <v>20</v>
+      </c>
+      <c r="C229" s="4" t="str">
         <f>TEXT( "      &lt;/cycle_macro&gt;", "=" )</f>
         <v xml:space="preserve">      &lt;/cycle_macro&gt;</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>229</v>
       </c>
-      <c r="B230" t="str">
+      <c r="B230">
+        <v>13</v>
+      </c>
+      <c r="C230" s="4" t="str">
         <f>TEXT( "    &lt;/macros&gt;", "=" )</f>
         <v xml:space="preserve">    &lt;/macros&gt;</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>230</v>
       </c>
-      <c r="B231" t="str">
+      <c r="B231">
+        <v>16</v>
+      </c>
+      <c r="C231" s="4" t="str">
         <f>TEXT( "  &lt;/definitions&gt;", "=" )</f>
         <v xml:space="preserve">  &lt;/definitions&gt;</v>
       </c>

</xml_diff>

<commit_message>
.gitignore .pyc => *.pyc
</commit_message>
<xml_diff>
--- a/data/short.xlsx
+++ b/data/short.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="155">
   <si>
     <t>AMANZI: The Multi-Process HPC Simulator</t>
   </si>
@@ -109,34 +109,34 @@
     <t>Title</t>
   </si>
   <si>
+    <t>Data file</t>
+  </si>
+  <si>
+    <t>short.rst</t>
+  </si>
+  <si>
+    <t>Data path</t>
+  </si>
+  <si>
+    <t>/Users/dantopa/Documents/repos/GitHub/topa-development/data/</t>
+  </si>
+  <si>
+    <t>Lines read</t>
+  </si>
+  <si>
+    <t>Output file</t>
+  </si>
+  <si>
+    <t>short.xlsx</t>
+  </si>
+  <si>
+    <t>Output path</t>
+  </si>
+  <si>
+    <t>boo:</t>
+  </si>
+  <si>
     <t>Amanzi XML Input Specification (Version 2.3-draft)</t>
-  </si>
-  <si>
-    <t>Data file</t>
-  </si>
-  <si>
-    <t>short.rst</t>
-  </si>
-  <si>
-    <t>Data path</t>
-  </si>
-  <si>
-    <t>/Users/dantopa/Documents/repos/GitHub/topa-development/data/</t>
-  </si>
-  <si>
-    <t>Lines read</t>
-  </si>
-  <si>
-    <t>Output file</t>
-  </si>
-  <si>
-    <t>short.xlsx</t>
-  </si>
-  <si>
-    <t>Output path</t>
-  </si>
-  <si>
-    <t>boo:</t>
   </si>
   <si>
     <t>.. contents:: **Table of Contents**</t>
@@ -922,7 +922,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="3">
-        <v>43441.83227679371</v>
+        <v>43442.45485502221</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1099,29 +1099,26 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>231</v>
@@ -1129,23 +1126,23 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1184,7 @@
         <v>50</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>